<commit_message>
new animation, began work on converging section heat trans
</commit_message>
<xml_diff>
--- a/converging_section/converge_geom.xlsx
+++ b/converging_section/converge_geom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SRVB\Homes$\zhaoqido\Documents\APS 490\Nozzle Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SRVB\Homes$\zhaoqido\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,16 +21,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
+    <t xml:space="preserve">Upper </t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
   </si>
   <si>
-    <t>Down</t>
-  </si>
-  <si>
-    <t>Up</t>
+    <t>Lower</t>
   </si>
 </sst>
 </file>
@@ -837,636 +837,606 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>-0.55990114599999996</v>
+        <v>4.2519685000000002E-2</v>
       </c>
       <c r="C2">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.0629921259999999</v>
       </c>
       <c r="E2">
-        <v>-0.582865262</v>
+        <v>4.2519685000000002E-2</v>
       </c>
       <c r="F2">
-        <v>8.8915102999999995E-2</v>
+        <v>0.95677905900000004</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>-0.53076316000000001</v>
+        <v>1.433647E-2</v>
       </c>
       <c r="C3">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.1030401030000001</v>
       </c>
       <c r="E3">
-        <v>-0.55225146400000003</v>
+        <v>3.9297776999999999E-2</v>
       </c>
       <c r="F3">
-        <v>8.8915102999999995E-2</v>
+        <v>0.96137466999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>-0.50495522900000001</v>
+        <v>-2.0942257999999998E-2</v>
       </c>
       <c r="C4">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.1538384180000001</v>
       </c>
       <c r="E4">
-        <v>-0.52467876999999996</v>
+        <v>3.5526228E-2</v>
       </c>
       <c r="F4">
-        <v>8.8915102999999995E-2</v>
+        <v>0.96665483900000004</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>-0.47581724199999997</v>
+        <v>-5.9144862999999999E-2</v>
       </c>
       <c r="C5">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.2073220650000001</v>
       </c>
       <c r="E5">
-        <v>-0.49215877099999999</v>
+        <v>3.0623213E-2</v>
       </c>
       <c r="F5">
-        <v>8.8915102999999995E-2</v>
+        <v>0.974575093</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>-0.44917679700000002</v>
+        <v>-0.13308576899999999</v>
       </c>
       <c r="C6">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.3124672639999999</v>
       </c>
       <c r="E6">
-        <v>-0.461284413</v>
+        <v>2.6851664000000001E-2</v>
       </c>
       <c r="F6">
-        <v>8.8915102999999995E-2</v>
+        <v>0.98155245899999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>-0.41421121300000002</v>
+        <v>-0.20613701400000001</v>
       </c>
       <c r="C7">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E7">
-        <v>-0.43222619400000001</v>
+        <v>2.2891537E-2</v>
       </c>
       <c r="F7">
-        <v>8.8915102999999995E-2</v>
+        <v>0.98947271299999995</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>-0.42488513700000002</v>
+        <v>-0.43081033499999999</v>
       </c>
       <c r="C8">
-        <v>-6.8989758999999998E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E8">
-        <v>-0.41134821799999999</v>
+        <v>1.7799945000000001E-2</v>
       </c>
       <c r="F8">
-        <v>9.0258673999999997E-2</v>
+        <v>0.99965589700000002</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>-0.39090082399999998</v>
+        <v>-0.61270137800000002</v>
       </c>
       <c r="C9">
-        <v>-5.9874937000000003E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E9">
-        <v>-0.39580441199999999</v>
+        <v>1.3085507999999999E-2</v>
       </c>
       <c r="F9">
-        <v>9.4758197000000002E-2</v>
+        <v>1.009273348</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>-0.37444334499999998</v>
+        <v>-0.897719088</v>
       </c>
       <c r="C10">
-        <v>-5.0476064000000001E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E10">
-        <v>-0.38176044799999997</v>
+        <v>9.2523789999999998E-3</v>
       </c>
       <c r="F10">
-        <v>0.102257401</v>
+        <v>1.021290743</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>-0.35843278200000001</v>
+        <v>-1.320201065</v>
       </c>
       <c r="C11">
-        <v>-3.8229576000000001E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E11">
-        <v>-0.36948902300000003</v>
+        <v>6.9421939999999996E-3</v>
       </c>
       <c r="F11">
-        <v>0.11248358899999999</v>
+        <v>1.028661332</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>-0.34971173999999999</v>
+        <v>-2.0383011930000001</v>
       </c>
       <c r="C12">
-        <v>-3.1348032999999997E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E12">
-        <v>-0.35843278200000001</v>
+        <v>4.411992E-3</v>
       </c>
       <c r="F12">
-        <v>0.122680818</v>
+        <v>1.036691974</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>-0.34296150800000003</v>
+        <v>-2.742356799</v>
       </c>
       <c r="C13">
-        <v>-2.6097852000000001E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E13">
-        <v>-0.347306481</v>
+        <v>1.9917989999999998E-3</v>
       </c>
       <c r="F13">
-        <v>0.13431305900000001</v>
+        <v>1.0439525540000001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>-0.33506892199999999</v>
+        <v>-3.4890107530000001</v>
       </c>
       <c r="C14">
-        <v>-2.0847671000000002E-2</v>
+        <v>1.4158897640000001</v>
       </c>
       <c r="E14">
-        <v>-0.33506892199999999</v>
+        <v>-8.6843E-4</v>
       </c>
       <c r="F14">
-        <v>0.14742527799999999</v>
+        <v>1.052093205</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>-0.32833600400000001</v>
-      </c>
-      <c r="C15">
-        <v>-1.5034970999999999E-2</v>
-      </c>
       <c r="E15">
-        <v>-0.32569118699999999</v>
+        <v>-3.398632E-3</v>
       </c>
       <c r="F15">
-        <v>0.156917786</v>
+        <v>1.0589137500000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>-0.32252330400000001</v>
-      </c>
-      <c r="C16">
-        <v>-9.5972839999999993E-3</v>
-      </c>
       <c r="E16">
-        <v>-0.31709073599999998</v>
+        <v>-8.7890629999999997E-3</v>
       </c>
       <c r="F16">
-        <v>0.16517325299999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>-0.315023045</v>
-      </c>
-      <c r="C17">
-        <v>-3.0345580000000001E-3</v>
-      </c>
+        <v>1.06716441</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17">
-        <v>-0.30757696200000001</v>
+        <v>-1.5216772E-2</v>
       </c>
       <c r="F17">
-        <v>0.1749559</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>-0.309210345</v>
-      </c>
-      <c r="C18">
-        <v>1.4655969999999999E-3</v>
-      </c>
+        <v>1.0729492549999999</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18">
-        <v>-0.296388765</v>
+        <v>-2.4644564000000001E-2</v>
       </c>
       <c r="F18">
-        <v>0.18629631899999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>-0.302272606</v>
-      </c>
-      <c r="C19">
-        <v>7.0907909999999999E-3</v>
-      </c>
+        <v>1.079009978</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19">
-        <v>-0.28685436600000003</v>
+        <v>-3.3847885000000001E-2</v>
       </c>
       <c r="F19">
-        <v>0.19587823200000001</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>-0.29570987999999998</v>
-      </c>
-      <c r="C20">
-        <v>1.3278504E-2</v>
-      </c>
+        <v>1.0821525759999999</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20">
-        <v>-0.27525274300000002</v>
+        <v>-4.6399904999999998E-2</v>
       </c>
       <c r="F20">
-        <v>0.20729273200000001</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>-0.288209622</v>
-      </c>
-      <c r="C21">
-        <v>1.9278711E-2</v>
-      </c>
+        <v>1.082872654</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21">
-        <v>-0.26458673500000002</v>
+        <v>-5.7041919000000003E-2</v>
       </c>
       <c r="F21">
-        <v>0.217771617</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>-0.27939681799999999</v>
-      </c>
-      <c r="C22">
-        <v>2.7153982E-2</v>
-      </c>
+        <v>1.082872654</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22">
-        <v>-0.254107851</v>
+        <v>-7.0773551000000004E-2</v>
       </c>
       <c r="F22">
-        <v>0.22825050199999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>-0.26983698900000003</v>
-      </c>
-      <c r="C23">
-        <v>3.6233044999999998E-2</v>
-      </c>
+        <v>1.080469619</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23">
-        <v>-0.244564118</v>
+        <v>-8.5878344999999995E-2</v>
       </c>
       <c r="F23">
-        <v>0.23741952699999999</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>-0.25622852000000002</v>
-      </c>
-      <c r="C24">
-        <v>4.8221458000000002E-2</v>
-      </c>
+        <v>1.077723293</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24">
-        <v>-0.233140973</v>
+        <v>-9.7550232000000001E-2</v>
       </c>
       <c r="F24">
-        <v>0.249021149</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>-0.244564118</v>
-      </c>
-      <c r="C25">
-        <v>6.0857893000000003E-2</v>
-      </c>
+        <v>1.0746336750000001</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25">
-        <v>-0.22062931</v>
+        <v>-0.112311736</v>
       </c>
       <c r="F25">
-        <v>0.26252468899999998</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>-0.233140973</v>
-      </c>
-      <c r="C26">
-        <v>7.1634505000000001E-2</v>
-      </c>
+        <v>1.0684544410000001</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26">
-        <v>-0.21120392900000001</v>
+        <v>-0.123983623</v>
       </c>
       <c r="F26">
-        <v>0.27287183999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>-0.223801483</v>
-      </c>
-      <c r="C27">
-        <v>8.1899178000000003E-2</v>
-      </c>
+        <v>1.062618498</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27">
-        <v>-0.199072951</v>
+        <v>-0.13771525500000001</v>
       </c>
       <c r="F27">
-        <v>0.28354233899999998</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>-0.21120392900000001</v>
-      </c>
-      <c r="C28">
-        <v>9.3097003999999997E-2</v>
-      </c>
+        <v>1.055409391</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28">
-        <v>-0.18603102599999999</v>
+        <v>-0.15007372299999999</v>
       </c>
       <c r="F28">
-        <v>0.29550623100000001</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>-0.199072951</v>
-      </c>
-      <c r="C29">
-        <v>0.106161134</v>
-      </c>
+        <v>1.046827121</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E29">
-        <v>-0.176833453</v>
+        <v>-0.160372447</v>
       </c>
       <c r="F29">
-        <v>0.30326730099999999</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>-0.188341701</v>
-      </c>
-      <c r="C30">
-        <v>0.11782553599999999</v>
-      </c>
+        <v>1.039274724</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E30">
-        <v>-0.16933804499999999</v>
+        <v>-0.17032787999999999</v>
       </c>
       <c r="F30">
-        <v>0.309191092</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>-0.18096262099999999</v>
-      </c>
-      <c r="C31">
-        <v>0.12522354399999999</v>
-      </c>
+        <v>1.029662582</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E31">
-        <v>-0.16141950799999999</v>
+        <v>-0.17992883600000001</v>
       </c>
       <c r="F31">
-        <v>0.31493354200000001</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>-0.17388062700000001</v>
-      </c>
-      <c r="C32">
-        <v>0.13303189600000001</v>
-      </c>
+        <v>1.020419239</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32">
-        <v>-0.15422633399999999</v>
+        <v>-0.188904459</v>
       </c>
       <c r="F32">
-        <v>0.31874169299999999</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>-0.16661704399999999</v>
-      </c>
-      <c r="C33">
-        <v>0.14047706900000001</v>
-      </c>
+        <v>1.0117331519999999</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33">
-        <v>-0.14252879900000001</v>
+        <v>-0.19527425600000001</v>
       </c>
       <c r="F33">
-        <v>0.32503949599999998</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>-0.15971663999999999</v>
-      </c>
-      <c r="C34">
-        <v>0.14864859999999999</v>
-      </c>
+        <v>1.004784283</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34">
-        <v>-0.12594097700000001</v>
+        <v>-0.20251266100000001</v>
       </c>
       <c r="F34">
-        <v>0.33232051899999998</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>-0.151363519</v>
-      </c>
-      <c r="C35">
-        <v>0.15754649000000001</v>
-      </c>
+        <v>0.99754587800000005</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E35">
-        <v>-0.13404854899999999</v>
+        <v>-0.20859292099999999</v>
       </c>
       <c r="F35">
-        <v>0.32940810999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>-0.14409993500000001</v>
-      </c>
-      <c r="C36">
-        <v>0.16517325299999999</v>
-      </c>
+        <v>0.99146561700000002</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E36">
-        <v>-0.114860913</v>
+        <v>-0.21467318199999999</v>
       </c>
       <c r="F36">
-        <v>0.33574688200000002</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>-0.13774429999999999</v>
-      </c>
-      <c r="C37">
-        <v>0.17152888799999999</v>
-      </c>
+        <v>0.985674893</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E37">
-        <v>-0.10535275400000001</v>
+        <v>-0.22162205099999999</v>
       </c>
       <c r="F37">
-        <v>0.33831665500000002</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>-0.13229661200000001</v>
-      </c>
-      <c r="C38">
-        <v>0.177521345</v>
-      </c>
+        <v>0.97872602399999997</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E38">
-        <v>-9.3017844000000002E-2</v>
+        <v>-0.23088721000000001</v>
       </c>
       <c r="F38">
-        <v>0.34020115499999998</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>-0.12594097700000001</v>
-      </c>
-      <c r="C39">
-        <v>0.18424015899999999</v>
-      </c>
+        <v>0.96975040099999998</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E39">
-        <v>-8.0559213000000005E-2</v>
+        <v>-0.23783607900000001</v>
       </c>
       <c r="F39">
-        <v>0.34221077900000002</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>-0.117517385</v>
-      </c>
-      <c r="C40">
-        <v>0.19339049999999999</v>
-      </c>
+        <v>0.96251199600000004</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E40">
-        <v>-6.7157977999999993E-2</v>
+        <v>-0.24796984699999999</v>
       </c>
       <c r="F40">
-        <v>0.34274563899999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>-0.109416324</v>
-      </c>
-      <c r="C41">
-        <v>0.199856864</v>
-      </c>
+        <v>0.95237822800000005</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E41">
-        <v>-5.3769149000000002E-2</v>
+        <v>-0.25636639700000002</v>
       </c>
       <c r="F41">
-        <v>0.34100509099999998</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>-9.9973666000000003E-2</v>
-      </c>
-      <c r="C42">
-        <v>0.20239911799999999</v>
-      </c>
+        <v>0.94485028699999996</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E42">
-        <v>-4.5233770999999999E-2</v>
+        <v>-0.26302573000000001</v>
       </c>
       <c r="F42">
-        <v>0.33765788400000002</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>-9.0349418000000001E-2</v>
-      </c>
-      <c r="C43">
-        <v>0.198404147</v>
-      </c>
+        <v>0.93819095399999997</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E43">
-        <v>-3.8204636E-2</v>
+        <v>-0.27142228000000002</v>
       </c>
       <c r="F43">
-        <v>0.33313915399999999</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>-8.3630602999999998E-2</v>
-      </c>
-      <c r="C44">
-        <v>0.188779899</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>-7.9090862999999997E-2</v>
-      </c>
-      <c r="C45">
-        <v>0.17988200900000001</v>
+        <v>0.93037347599999998</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>-0.280397903</v>
+      </c>
+      <c r="F44">
+        <v>0.92168738900000002</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>-0.290821206</v>
+      </c>
+      <c r="F45">
+        <v>0.91126408599999997</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>-0.29805961199999997</v>
+      </c>
+      <c r="F46">
+        <v>0.90489428900000002</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>-0.30848291500000002</v>
+      </c>
+      <c r="F47">
+        <v>0.89533959399999996</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>-0.31716900199999998</v>
+      </c>
+      <c r="F48">
+        <v>0.88781165200000001</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>-0.32382833500000002</v>
+      </c>
+      <c r="F49">
+        <v>0.88202092799999998</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>-0.33135627600000001</v>
+      </c>
+      <c r="F50">
+        <v>0.87507205899999996</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>-0.33743653699999998</v>
+      </c>
+      <c r="F51">
+        <v>0.869860407</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>-0.34351679699999998</v>
+      </c>
+      <c r="F52">
+        <v>0.86464875500000005</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>-0.35162381100000001</v>
+      </c>
+      <c r="F53">
+        <v>0.86030571199999994</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>-0.36696350900000002</v>
+      </c>
+      <c r="F54">
+        <v>0.85691813299999997</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>-0.43898398199999999</v>
+      </c>
+      <c r="F55">
+        <v>0.85691815000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>-0.66303869100000001</v>
+      </c>
+      <c r="F56">
+        <v>0.85691815000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>-0.91623872799999995</v>
+      </c>
+      <c r="F57">
+        <v>0.85691815000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>-1.1543650839999999</v>
+      </c>
+      <c r="F58">
+        <v>0.85691815000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>-1.1543650839999999</v>
+      </c>
+      <c r="F59">
+        <v>0.95534334600000004</v>
+      </c>
+    </row>
+    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>-1.320201065</v>
+      </c>
+      <c r="F60">
+        <v>0.95677905900000004</v>
+      </c>
+    </row>
+    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>-2.0383011930000001</v>
+      </c>
+      <c r="F61">
+        <v>0.95677905900000004</v>
+      </c>
+    </row>
+    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>-2.742356799</v>
+      </c>
+      <c r="F62">
+        <v>0.95677905900000004</v>
+      </c>
+    </row>
+    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>-3.4664625689999999</v>
+      </c>
+      <c r="F63">
+        <v>0.95677905900000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>